<commit_message>
added delete to orders
</commit_message>
<xml_diff>
--- a/orders/123478.xlsx
+++ b/orders/123478.xlsx
@@ -14,7 +14,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>ManufacturerPart</t>
+  </si>
+  <si>
+    <t>ProcessRequest</t>
+  </si>
+  <si>
+    <t>SortingRequest</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>UnitPrice</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
   <si>
     <t>CZ-4180</t>
   </si>
@@ -893,51 +923,51 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -945,31 +975,31 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -977,31 +1007,31 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1009,31 +1039,31 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1041,31 +1071,31 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1073,31 +1103,31 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1105,31 +1135,31 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
       <c r="I8" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1137,31 +1167,31 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
       <c r="I9" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1169,31 +1199,31 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1201,31 +1231,31 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1233,31 +1263,31 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -1265,31 +1295,31 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1297,31 +1327,31 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -1329,31 +1359,31 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
       <c r="I15" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -1361,31 +1391,31 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F16" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J16">
         <v>0</v>
@@ -1393,31 +1423,31 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F17" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1425,31 +1455,31 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1457,31 +1487,31 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G19" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -1489,31 +1519,31 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G20" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
       <c r="I20" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1521,31 +1551,31 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F21" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G21" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J21">
         <v>0</v>
@@ -1553,31 +1583,31 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F22" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G22" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1585,31 +1615,31 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="E23" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F23" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G23" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -1617,31 +1647,31 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -1649,31 +1679,31 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -1681,31 +1711,31 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G26" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1713,31 +1743,31 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E27" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F27" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G27" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -1745,31 +1775,31 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C28" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F28" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G28" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
       <c r="I28" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J28">
         <v>0</v>
@@ -1777,31 +1807,31 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F29" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G29" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
       <c r="I29" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J29">
         <v>0</v>
@@ -1809,31 +1839,31 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B30" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="E30" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F30" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G30" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J30">
         <v>0</v>
@@ -1841,31 +1871,31 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C31" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E31" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F31" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J31">
         <v>0</v>
@@ -1873,31 +1903,31 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C32" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D32" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F32" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G32" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -1905,31 +1935,31 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F33" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G33" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
       <c r="I33" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J33">
         <v>0</v>
@@ -1937,31 +1967,31 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E34" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F34" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G34" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
       <c r="I34" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J34">
         <v>0</v>
@@ -1969,31 +1999,31 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C35" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F35" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G35" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
       <c r="I35" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J35">
         <v>0</v>
@@ -2001,31 +2031,31 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C36" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F36" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G36" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H36">
         <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -2033,31 +2063,31 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D37" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E37" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F37" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G37" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -2065,31 +2095,31 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="E38" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F38" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G38" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J38">
         <v>0</v>
@@ -2097,31 +2127,31 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C39" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D39" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F39" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G39" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H39">
         <v>0</v>
       </c>
       <c r="I39" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J39">
         <v>0</v>
@@ -2129,31 +2159,31 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C40" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F40" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G40" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -2161,31 +2191,31 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C41" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D41" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E41" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F41" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
       <c r="I41" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -2193,31 +2223,31 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C42" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E42" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F42" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G42" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -2225,31 +2255,31 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C43" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E43" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F43" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
       <c r="I43" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J43">
         <v>0</v>
@@ -2257,31 +2287,31 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="B44" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C44" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="E44" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F44" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G44" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H44">
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J44">
         <v>0</v>
@@ -2289,31 +2319,31 @@
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="B45" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D45" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E45" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F45" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G45" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H45">
         <v>0</v>
       </c>
       <c r="I45" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -2321,31 +2351,31 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B46" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="E46" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F46" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G46" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
       <c r="I46" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J46">
         <v>0</v>
@@ -2353,31 +2383,31 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C47" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D47" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E47" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F47" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G47" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H47">
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J47">
         <v>0</v>
@@ -2385,31 +2415,31 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="B48" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C48" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E48" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F48" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G48" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J48">
         <v>0</v>
@@ -2417,31 +2447,31 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B49" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C49" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D49" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E49" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F49" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G49" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J49">
         <v>0</v>
@@ -2449,31 +2479,31 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E50" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F50" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G50" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
       <c r="I50" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J50">
         <v>0</v>
@@ -2481,31 +2511,31 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C51" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D51" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E51" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F51" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
       <c r="I51" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J51">
         <v>0</v>
@@ -2513,31 +2543,31 @@
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B52" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C52" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E52" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F52" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G52" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
       <c r="I52" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J52">
         <v>0</v>
@@ -2545,31 +2575,31 @@
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="B53" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C53" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D53" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="E53" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F53" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G53" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H53">
         <v>0</v>
       </c>
       <c r="I53" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J53">
         <v>0</v>
@@ -2577,31 +2607,31 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C54" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E54" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F54" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G54" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H54">
         <v>0</v>
       </c>
       <c r="I54" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J54">
         <v>0</v>
@@ -2609,31 +2639,31 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B55" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C55" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D55" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E55" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F55" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G55" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -2641,31 +2671,31 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D56" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="E56" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F56" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J56">
         <v>0</v>
@@ -2673,31 +2703,31 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="B57" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="E57" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F57" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J57">
         <v>0</v>
@@ -2705,31 +2735,31 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B58" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C58" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D58" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="E58" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F58" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
       <c r="H58">
-        <v>269</v>
+        <v>0</v>
       </c>
       <c r="I58" t="s">
-        <v>119</v>
+        <v>11</v>
       </c>
       <c r="J58">
         <v>0</v>
@@ -2737,127 +2767,127 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B59" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C59" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="E59" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="F59" t="s">
-        <v>122</v>
+        <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="H59">
-        <v>5.61</v>
+        <v>269</v>
       </c>
       <c r="I59" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="J59">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B60" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C60" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D60" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="E60" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F60" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G60" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="H60">
-        <v>5.17</v>
+        <v>5.61</v>
       </c>
       <c r="I60" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J60">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B61" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C61" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D61" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E61" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F61" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G61" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="H61">
-        <v>5.61</v>
+        <v>5.17</v>
       </c>
       <c r="I61" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J61">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C62" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D62" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E62" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F62" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G62" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="H62">
-        <v>5.17</v>
+        <v>5.61</v>
       </c>
       <c r="I62" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J62">
         <v>10</v>
@@ -2865,31 +2895,31 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B63" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C63" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
+        <v>140</v>
+      </c>
+      <c r="E63" t="s">
         <v>132</v>
       </c>
-      <c r="E63" t="s">
-        <v>122</v>
-      </c>
       <c r="F63" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G63" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="H63">
-        <v>5.61</v>
+        <v>5.17</v>
       </c>
       <c r="I63" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J63">
         <v>10</v>
@@ -2897,127 +2927,127 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>141</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>142</v>
+      </c>
+      <c r="E64" t="s">
+        <v>132</v>
+      </c>
+      <c r="F64" t="s">
+        <v>132</v>
+      </c>
+      <c r="G64" t="s">
         <v>133</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1</v>
-      </c>
-      <c r="C64" t="s">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s">
-        <v>134</v>
-      </c>
-      <c r="E64" t="s">
-        <v>122</v>
-      </c>
-      <c r="F64" t="s">
-        <v>122</v>
-      </c>
-      <c r="G64" t="s">
-        <v>123</v>
       </c>
       <c r="H64">
         <v>5.61</v>
       </c>
       <c r="I64" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J64">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="B65" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C65" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D65" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E65" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F65" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G65" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="H65">
-        <v>6.52</v>
+        <v>5.61</v>
       </c>
       <c r="I65" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J65">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B66" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C66" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E66" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="F66" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="G66" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="H66">
-        <v>9.09</v>
+        <v>6.52</v>
       </c>
       <c r="I66" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J66">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B67" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C67" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D67" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="E67" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F67" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G67" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="H67">
         <v>9.09</v>
       </c>
       <c r="I67" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J67">
         <v>4</v>
@@ -3025,63 +3055,63 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D68" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E68" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F68" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G68" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="H68">
-        <v>13</v>
+        <v>9.09</v>
       </c>
       <c r="I68" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J68">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B69" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="C69" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D69" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E69" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="F69" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="G69" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="H69">
         <v>13</v>
       </c>
       <c r="I69" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J69">
         <v>6</v>
@@ -3089,63 +3119,63 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B70" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C70" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="E70" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="F70" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="G70" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="H70">
-        <v>8.09</v>
+        <v>13</v>
       </c>
       <c r="I70" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J70">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C71" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D71" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="E71" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="F71" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="G71" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="H71">
         <v>8.09</v>
       </c>
       <c r="I71" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J71">
         <v>4</v>
@@ -3153,319 +3183,319 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B72" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C72" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D72" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E72" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="F72" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="G72" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="H72">
-        <v>8.48</v>
+        <v>8.09</v>
       </c>
       <c r="I72" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B73" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C73" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D73" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E73" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="F73" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="G73" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="H73">
         <v>8.48</v>
       </c>
       <c r="I73" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J73">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B74" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C74" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D74" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
       <c r="E74" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="F74" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="G74" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="H74">
-        <v>7.78</v>
+        <v>8.48</v>
       </c>
       <c r="I74" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J74">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B75" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C75" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D75" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E75" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="F75" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="G75" t="s">
-        <v>118</v>
+        <v>173</v>
       </c>
       <c r="H75">
-        <v>11.22</v>
+        <v>7.78</v>
       </c>
       <c r="I75" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J75">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="B76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" t="s">
+        <v>175</v>
+      </c>
+      <c r="E76" t="s">
+        <v>167</v>
+      </c>
+      <c r="F76" t="s">
+        <v>167</v>
+      </c>
+      <c r="G76" t="s">
+        <v>128</v>
+      </c>
+      <c r="H76">
+        <v>11.22</v>
+      </c>
+      <c r="I76" t="s">
+        <v>134</v>
+      </c>
+      <c r="J76">
         <v>1</v>
-      </c>
-      <c r="C76" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" t="s">
-        <v>167</v>
-      </c>
-      <c r="E76" t="s">
-        <v>137</v>
-      </c>
-      <c r="F76" t="s">
-        <v>137</v>
-      </c>
-      <c r="G76" t="s">
-        <v>168</v>
-      </c>
-      <c r="H76">
-        <v>7.78</v>
-      </c>
-      <c r="I76" t="s">
-        <v>124</v>
-      </c>
-      <c r="J76">
-        <v>6</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B77" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C77" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D77" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E77" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="F77" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="G77" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H77">
-        <v>10.39</v>
+        <v>7.78</v>
       </c>
       <c r="I77" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J77">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B78" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C78" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D78" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E78" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="F78" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="G78" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H78">
         <v>10.39</v>
       </c>
       <c r="I78" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J78">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B79" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C79" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D79" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="F79" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="G79" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H79">
         <v>10.39</v>
       </c>
       <c r="I79" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="J79">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B80" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D80" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E80" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="F80" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="G80" t="s">
         <v>178</v>
       </c>
       <c r="H80">
-        <v>80</v>
+        <v>10.39</v>
       </c>
       <c r="I80" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="J80">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B81" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C81" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D81" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="E81" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="F81" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G81" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="H81">
         <v>80</v>
       </c>
       <c r="I81" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="J81">
         <v>10</v>
@@ -3473,31 +3503,31 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B82" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C82" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D82" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="E82" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="F82" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G82" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="H82">
         <v>80</v>
       </c>
       <c r="I82" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="J82">
         <v>10</v>
@@ -3505,33 +3535,65 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B83" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C83" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D83" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E83" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="F83" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G83" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="H83">
         <v>80</v>
       </c>
       <c r="I83" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="J83">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>193</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" t="s">
+        <v>12</v>
+      </c>
+      <c r="D84" t="s">
+        <v>194</v>
+      </c>
+      <c r="E84" t="s">
+        <v>187</v>
+      </c>
+      <c r="F84" t="s">
+        <v>187</v>
+      </c>
+      <c r="G84" t="s">
+        <v>188</v>
+      </c>
+      <c r="H84">
+        <v>80</v>
+      </c>
+      <c r="I84" t="s">
+        <v>129</v>
+      </c>
+      <c r="J84">
         <v>10</v>
       </c>
     </row>

</xml_diff>